<commit_message>
Renamed SMM enum to SMHF
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/MastersResults-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/MastersResults-A4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A40C99C-71A4-416C-91E8-FDDAE44F74DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A131B6-8D68-408A-BDF3-50701FA4816C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="23625" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -224,9 +224,6 @@
     <t>${t.get("Results.Rank")}</t>
   </si>
   <si>
-    <t>${t.get("smm")}</t>
-  </si>
-  <si>
     <t>${t.get("Results.Sinclair")}</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>${r.resRecordLift}</t>
+  </si>
+  <si>
+    <t>${t.get("smhf")}</t>
   </si>
 </sst>
 </file>
@@ -311,9 +311,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0;;"/>
-    <numFmt numFmtId="166" formatCode="0;\(0\);\-"/>
-    <numFmt numFmtId="167" formatCode="0.000;;\-"/>
-    <numFmt numFmtId="168" formatCode="0;;\-;@"/>
+    <numFmt numFmtId="165" formatCode="0;\(0\);\-"/>
+    <numFmt numFmtId="166" formatCode="0.000;;\-"/>
+    <numFmt numFmtId="167" formatCode="0;;\-;@"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -842,27 +842,27 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1048,18 +1048,34 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1079,22 +1095,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1690,7 +1690,7 @@
         <v>36</v>
       </c>
       <c r="K3" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L3" s="32"/>
       <c r="M3" s="33"/>
@@ -1750,33 +1750,33 @@
       <c r="H6" s="47"/>
       <c r="I6" s="5"/>
       <c r="J6" s="47"/>
-      <c r="K6" s="89" t="s">
+      <c r="K6" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="90"/>
-      <c r="M6" s="91"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="92"/>
       <c r="N6" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="89" t="s">
+      <c r="O6" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="91"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="92"/>
       <c r="R6" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="94" t="s">
+      <c r="S6" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="T6" s="92" t="s">
+      <c r="T6" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="U6" s="96" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6" s="98" t="s">
+      <c r="U6" s="100" t="s">
         <v>54</v>
+      </c>
+      <c r="V6" s="89" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1792,10 +1792,10 @@
       <c r="D7" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="89" t="s">
+      <c r="E7" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="91"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="52" t="s">
         <v>48</v>
       </c>
@@ -1830,12 +1830,12 @@
         <v>3</v>
       </c>
       <c r="R7" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="S7" s="95"/>
-      <c r="T7" s="93"/>
-      <c r="U7" s="97"/>
-      <c r="V7" s="99"/>
+        <v>55</v>
+      </c>
+      <c r="S7" s="99"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="101"/>
+      <c r="V7" s="90"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1872,10 +1872,10 @@
       <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="101"/>
+      <c r="F9" s="94"/>
       <c r="G9" s="19" t="s">
         <v>31</v>
       </c>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="13" spans="1:24" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J13" s="22"/>
     </row>
@@ -2021,28 +2021,28 @@
     </row>
     <row r="15" spans="1:24" s="70" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A15" s="61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="62"/>
       <c r="C15" s="63"/>
       <c r="D15" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="65" t="s">
         <v>61</v>
-      </c>
-      <c r="E15" s="65" t="s">
-        <v>62</v>
       </c>
       <c r="F15" s="64" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="67"/>
       <c r="I15" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="61" t="s">
         <v>64</v>
-      </c>
-      <c r="J15" s="61" t="s">
-        <v>65</v>
       </c>
       <c r="K15" s="68"/>
       <c r="L15" s="62"/>
@@ -2057,18 +2057,18 @@
       </c>
       <c r="R15" s="62"/>
       <c r="S15" s="61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T15" s="68"/>
       <c r="U15" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V15" s="69"/>
       <c r="X15" s="63"/>
     </row>
     <row r="16" spans="1:24" s="75" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" s="72"/>
@@ -2084,47 +2084,47 @@
     </row>
     <row r="17" spans="1:24" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="77"/>
       <c r="C17" s="78"/>
       <c r="D17" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="80" t="s">
-        <v>71</v>
-      </c>
       <c r="F17" s="88" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="78"/>
       <c r="I17" s="87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" s="80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K17" s="77"/>
       <c r="L17" s="77"/>
       <c r="M17" s="78"/>
       <c r="N17" s="80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O17" s="77"/>
       <c r="P17" s="78"/>
       <c r="Q17" s="76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R17" s="77"/>
       <c r="S17" s="81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T17" s="77"/>
       <c r="U17" s="82" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V17" s="78"/>
       <c r="X17" s="78"/>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="19" spans="1:24" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="72"/>

</xml_diff>